<commit_message>
show only the test created by a user
</commit_message>
<xml_diff>
--- a/credenziali.xlsx
+++ b/credenziali.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +52,9 @@
   <si>
     <t>docente</t>
   </si>
+  <si>
+    <t>marco</t>
+  </si>
 </sst>
 </file>
 
@@ -63,7 +66,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +76,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -555,157 +551,160 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1030,13 +1029,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="D5:F8"/>
+  <dimension ref="D5:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.95" outlineLevelRow="7" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.95" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
     <col min="4" max="5" width="17.9719626168224" style="1" customWidth="1"/>
@@ -1088,6 +1087,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="4:6">
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>